<commit_message>
Added choosing of which excel file to edit.
</commit_message>
<xml_diff>
--- a/record_data/ivan-records.xlsx
+++ b/record_data/ivan-records.xlsx
@@ -380,7 +380,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H179"/>
+  <dimension ref="A1:H181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
       <selection activeCell="B175" sqref="B175"/>
@@ -6290,7 +6290,6 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="inlineStr"/>
       <c r="B179" t="inlineStr">
         <is>
           <t>Pianoman</t>
@@ -6321,6 +6320,73 @@
       </c>
       <c r="H179" t="n">
         <v>1.69</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Untitled (5)</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Four Flies</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>EP</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>House, Drum n Bass</t>
+        </is>
+      </c>
+      <c r="F180" t="n">
+        <v>2003</v>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="H180" t="n">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr"/>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>E'voke</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Runaway</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>EP</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>Progressive House, House</t>
+        </is>
+      </c>
+      <c r="F181" t="n">
+        <v>1995</v>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="H181" t="n">
+        <v>3.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>